<commit_message>
湖北 2.19 2.20 更新
</commit_message>
<xml_diff>
--- a/data/unchecked/manual_collect/china/hubei/hubeiCaseStatistics_20200219.xlsx
+++ b/data/unchecked/manual_collect/china/hubei/hubeiCaseStatistics_20200219.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huawei\Desktop\疫情大数据\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5B026F2-4ED0-44A1-BF8F-4A983492D168}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDAF4B17-E254-4A93-9567-373CEB1D2602}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13300" yWindow="-60" windowWidth="16200" windowHeight="10060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="新数据表" sheetId="1" r:id="rId1"/>
@@ -383,7 +383,7 @@
     <definedName name="自贡市">中国各省市区县数据!$C$2043:$C$2048</definedName>
     <definedName name="遵义市">中国各省市区县数据!$C$2220:$C$2233</definedName>
   </definedNames>
-  <calcPr calcId="181029" concurrentCalc="0"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -10805,18 +10805,19 @@
   <dimension ref="A1:AN27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="5" topLeftCell="Q1" activePane="topRight" state="frozen"/>
+      <pane xSplit="5" topLeftCell="H1" activePane="topRight" state="frozen"/>
       <selection activeCell="G1" sqref="G1"/>
-      <selection pane="topRight" activeCell="Q2" sqref="Q2:Q19"/>
+      <selection pane="topRight" activeCell="G23" activeCellId="1" sqref="A19:XFD19 G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.84375" defaultRowHeight="16.5"/>
   <cols>
-    <col min="1" max="2" width="14.84375" style="13" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="14.84375" style="15" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="14.84375" style="13" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="4.61328125" style="13" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="6.3046875" style="13" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="14.84375" style="13" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="8" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.84375" style="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.84375" style="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.61328125" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.3046875" style="13" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.61328125" style="13" customWidth="1"/>
     <col min="8" max="8" width="16.15234375" style="13" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="12.4609375" style="13" bestFit="1" customWidth="1"/>
@@ -11070,6 +11071,9 @@
       <c r="G3" s="19" t="s">
         <v>257</v>
       </c>
+      <c r="I3" s="13">
+        <v>66</v>
+      </c>
       <c r="K3" s="13">
         <v>101</v>
       </c>
@@ -11077,16 +11081,13 @@
         <v>7</v>
       </c>
       <c r="M3" s="13">
-        <v>3329</v>
+        <v>3410</v>
       </c>
       <c r="N3" s="12"/>
       <c r="O3" s="12"/>
       <c r="P3" s="13">
         <v>89</v>
       </c>
-      <c r="Q3" s="13">
-        <v>-15</v>
-      </c>
       <c r="S3" s="13" t="s">
         <v>3288</v>
       </c>
@@ -11144,6 +11145,9 @@
       <c r="G4" s="19" t="s">
         <v>307</v>
       </c>
+      <c r="I4" s="13">
+        <v>22</v>
+      </c>
       <c r="K4" s="13">
         <v>90</v>
       </c>
@@ -11151,16 +11155,13 @@
         <v>2</v>
       </c>
       <c r="M4" s="12">
-        <v>2839</v>
+        <v>2866</v>
       </c>
       <c r="N4" s="12"/>
       <c r="O4" s="12"/>
       <c r="P4" s="13">
         <v>87</v>
       </c>
-      <c r="Q4" s="13">
-        <v>-5</v>
-      </c>
       <c r="S4" s="13" t="s">
         <v>3288</v>
       </c>
@@ -11219,7 +11220,7 @@
         <v>351</v>
       </c>
       <c r="I5" s="13">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="K5" s="13">
         <v>54</v>
@@ -11228,7 +11229,7 @@
         <v>1</v>
       </c>
       <c r="M5" s="12">
-        <v>1283</v>
+        <v>1288</v>
       </c>
       <c r="N5" s="12"/>
       <c r="O5" s="12"/>
@@ -11292,6 +11293,9 @@
       <c r="G6" s="19" t="s">
         <v>283</v>
       </c>
+      <c r="I6" s="13">
+        <v>12</v>
+      </c>
       <c r="K6" s="13">
         <v>42</v>
       </c>
@@ -11299,16 +11303,13 @@
         <v>2</v>
       </c>
       <c r="M6" s="12">
-        <v>1510</v>
+        <v>1553</v>
       </c>
       <c r="N6" s="12"/>
       <c r="O6" s="12"/>
       <c r="P6" s="13">
         <v>40</v>
       </c>
-      <c r="Q6" s="13">
-        <v>-31</v>
-      </c>
       <c r="S6" s="13" t="s">
         <v>3288</v>
       </c>
@@ -11367,7 +11368,7 @@
         <v>172</v>
       </c>
       <c r="I7" s="13">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K7" s="13">
         <v>64</v>
@@ -11376,7 +11377,7 @@
         <v>1</v>
       </c>
       <c r="M7" s="12">
-        <v>1167</v>
+        <v>1168</v>
       </c>
       <c r="N7" s="12"/>
       <c r="O7" s="12"/>
@@ -11440,6 +11441,9 @@
       <c r="G8" s="19" t="s">
         <v>85</v>
       </c>
+      <c r="I8" s="13">
+        <v>2</v>
+      </c>
       <c r="K8" s="13">
         <v>37</v>
       </c>
@@ -11447,16 +11451,13 @@
         <v>1</v>
       </c>
       <c r="M8" s="12">
-        <v>967</v>
+        <v>985</v>
       </c>
       <c r="N8" s="12"/>
       <c r="O8" s="12"/>
       <c r="P8" s="13">
         <v>26</v>
       </c>
-      <c r="Q8" s="13">
-        <v>-16</v>
-      </c>
       <c r="S8" s="13" t="s">
         <v>3288</v>
       </c>
@@ -11514,6 +11515,9 @@
       <c r="G9" s="19" t="s">
         <v>143</v>
       </c>
+      <c r="I9" s="13">
+        <v>3</v>
+      </c>
       <c r="K9" s="13">
         <v>23</v>
       </c>
@@ -11521,16 +11525,13 @@
         <v>2</v>
       </c>
       <c r="M9" s="12">
-        <v>891</v>
+        <v>910</v>
       </c>
       <c r="N9" s="12"/>
       <c r="O9" s="12"/>
       <c r="P9" s="13">
         <v>27</v>
       </c>
-      <c r="Q9" s="13">
-        <v>-16</v>
-      </c>
       <c r="S9" s="13" t="s">
         <v>3288</v>
       </c>
@@ -11588,6 +11589,9 @@
       <c r="G10" s="19" t="s">
         <v>229</v>
       </c>
+      <c r="I10" s="13">
+        <v>5</v>
+      </c>
       <c r="K10" s="13">
         <v>20</v>
       </c>
@@ -11595,16 +11599,13 @@
         <v>1</v>
       </c>
       <c r="M10" s="12">
-        <v>794</v>
+        <v>906</v>
       </c>
       <c r="N10" s="12"/>
       <c r="O10" s="12"/>
       <c r="P10" s="13">
         <v>34</v>
       </c>
-      <c r="Q10" s="13">
-        <v>-107</v>
-      </c>
       <c r="S10" s="13" t="s">
         <v>3288</v>
       </c>
@@ -11662,6 +11663,9 @@
       <c r="G11" s="19" t="s">
         <v>201</v>
       </c>
+      <c r="I11" s="13">
+        <v>25</v>
+      </c>
       <c r="K11" s="13">
         <v>49</v>
       </c>
@@ -11669,16 +11673,13 @@
         <v>1</v>
       </c>
       <c r="M11" s="12">
-        <v>1338</v>
+        <v>1368</v>
       </c>
       <c r="N11" s="12"/>
       <c r="O11" s="12"/>
       <c r="P11" s="13">
         <v>38</v>
       </c>
-      <c r="Q11" s="13">
-        <v>-5</v>
-      </c>
       <c r="S11" s="13" t="s">
         <v>3288</v>
       </c>
@@ -11736,20 +11737,20 @@
       <c r="G12" s="19" t="s">
         <v>330</v>
       </c>
+      <c r="I12" s="13">
+        <v>2</v>
+      </c>
       <c r="K12" s="13">
         <v>43</v>
       </c>
       <c r="M12" s="12">
-        <v>766</v>
+        <v>834</v>
       </c>
       <c r="N12" s="12"/>
       <c r="O12" s="12"/>
       <c r="P12" s="13">
         <v>10</v>
       </c>
-      <c r="Q12" s="13">
-        <v>-66</v>
-      </c>
       <c r="S12" s="13" t="s">
         <v>3288</v>
       </c>
@@ -11808,13 +11809,13 @@
         <v>114</v>
       </c>
       <c r="I13" s="13">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="K13" s="13">
         <v>23</v>
       </c>
       <c r="M13" s="12">
-        <v>641</v>
+        <v>643</v>
       </c>
       <c r="N13" s="12"/>
       <c r="O13" s="12"/>
@@ -11949,6 +11950,9 @@
       <c r="G15" s="19" t="s">
         <v>407</v>
       </c>
+      <c r="I15" s="13">
+        <v>2</v>
+      </c>
       <c r="K15" s="13">
         <v>60</v>
       </c>
@@ -11956,16 +11960,13 @@
         <v>1</v>
       </c>
       <c r="M15" s="12">
-        <v>473</v>
+        <v>488</v>
       </c>
       <c r="N15" s="12"/>
       <c r="O15" s="12"/>
       <c r="P15" s="13">
         <v>12</v>
       </c>
-      <c r="Q15" s="13">
-        <v>-13</v>
-      </c>
       <c r="S15" s="13" t="s">
         <v>3288</v>
       </c>
@@ -12027,15 +12028,12 @@
         <v>6</v>
       </c>
       <c r="M16" s="12">
-        <v>244</v>
+        <v>249</v>
       </c>
       <c r="N16" s="12"/>
       <c r="O16" s="12"/>
       <c r="P16" s="13">
         <v>3</v>
-      </c>
-      <c r="Q16" s="13">
-        <v>-5</v>
       </c>
       <c r="S16" s="13" t="s">
         <v>3288</v>
@@ -12287,7 +12285,7 @@
       <c r="G20" s="19"/>
       <c r="I20" s="13">
         <f>SUM(I2:I19)</f>
-        <v>628</v>
+        <v>775</v>
       </c>
       <c r="J20" s="13">
         <v>-6</v>
@@ -12302,7 +12300,7 @@
       </c>
       <c r="M20" s="13">
         <f>SUM(M2:M19)</f>
-        <v>62031</v>
+        <v>62457</v>
       </c>
       <c r="N20" s="13">
         <v>3456</v>
@@ -12316,10 +12314,10 @@
       </c>
       <c r="Q20" s="13">
         <f>SUM(Q2:Q18)</f>
-        <v>-279</v>
+        <v>0</v>
       </c>
       <c r="R20" s="13">
-        <v>-1411</v>
+        <v>-1132</v>
       </c>
       <c r="S20" s="13" t="s">
         <v>3288</v>

</xml_diff>